<commit_message>
Update to calculate scores relative to median AFTER merging with zip/census tract
</commit_message>
<xml_diff>
--- a/data/children_in_poverty_100_fpl.xlsx
+++ b/data/children_in_poverty_100_fpl.xlsx
@@ -391,11 +391,11 @@
         </is>
       </c>
       <c r="C2">
-        <v>1.443877551020408</v>
+        <v>0.7251761691223575</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -411,11 +411,11 @@
         </is>
       </c>
       <c r="C3">
-        <v>1.831632653061224</v>
+        <v>0.9199231262011531</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>5.292857142857143</v>
+        <v>2.65829596412556</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -451,11 +451,11 @@
         </is>
       </c>
       <c r="C5">
-        <v>4.035714285714286</v>
+        <v>2.026905829596413</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>6.24404761904762</v>
+        <v>3.136023916292975</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>4.836734693877551</v>
+        <v>2.429212043561819</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -511,11 +511,11 @@
         </is>
       </c>
       <c r="C8">
-        <v>3.178571428571428</v>
+        <v>1.596412556053812</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>8.642857142857142</v>
+        <v>4.340807174887892</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -551,11 +551,11 @@
         </is>
       </c>
       <c r="C10">
-        <v>1.25</v>
+        <v>0.6278026905829597</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -571,11 +571,11 @@
         </is>
       </c>
       <c r="C11">
-        <v>1.517857142857143</v>
+        <v>0.7623318385650224</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -591,11 +591,11 @@
         </is>
       </c>
       <c r="C12">
-        <v>1.683673469387755</v>
+        <v>0.8456117873158232</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -611,11 +611,11 @@
         </is>
       </c>
       <c r="C13">
-        <v>1.955357142857143</v>
+        <v>0.9820627802690582</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="C14">
-        <v>1.955357142857143</v>
+        <v>0.9820627802690582</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -651,11 +651,11 @@
         </is>
       </c>
       <c r="C15">
-        <v>1.791666666666667</v>
+        <v>0.8998505231689088</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -671,11 +671,11 @@
         </is>
       </c>
       <c r="C16">
-        <v>2.164285714285714</v>
+        <v>1.086995515695067</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -691,11 +691,11 @@
         </is>
       </c>
       <c r="C17">
-        <v>2.09375</v>
+        <v>1.051569506726457</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -711,11 +711,11 @@
         </is>
       </c>
       <c r="C18">
-        <v>2.464285714285714</v>
+        <v>1.237668161434978</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -731,11 +731,11 @@
         </is>
       </c>
       <c r="C19">
-        <v>1.813492063492063</v>
+        <v>0.9108121574489287</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -751,11 +751,11 @@
         </is>
       </c>
       <c r="C20">
-        <v>1.511904761904762</v>
+        <v>0.7593423019431988</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -771,11 +771,11 @@
         </is>
       </c>
       <c r="C21">
-        <v>1.571428571428571</v>
+        <v>0.7892376681614349</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -791,11 +791,11 @@
         </is>
       </c>
       <c r="C22">
-        <v>1.770408163265306</v>
+        <v>0.8891736066623959</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -811,11 +811,11 @@
         </is>
       </c>
       <c r="C23">
-        <v>1.668367346938775</v>
+        <v>0.8379244074311339</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="C24">
-        <v>5.764285714285714</v>
+        <v>2.895067264573991</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="C25">
-        <v>3.576530612244898</v>
+        <v>1.796284433055733</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C26">
-        <v>6.011904761904762</v>
+        <v>3.019431988041854</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -891,11 +891,11 @@
         </is>
       </c>
       <c r="C27">
-        <v>2.910714285714286</v>
+        <v>1.461883408071749</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -911,11 +911,11 @@
         </is>
       </c>
       <c r="C28">
-        <v>4.232142857142857</v>
+        <v>2.125560538116592</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -931,11 +931,11 @@
         </is>
       </c>
       <c r="C29">
-        <v>1.921428571428571</v>
+        <v>0.9650224215246637</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -951,11 +951,11 @@
         </is>
       </c>
       <c r="C30">
-        <v>4.160714285714286</v>
+        <v>2.089686098654708</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -971,11 +971,11 @@
         </is>
       </c>
       <c r="C31">
-        <v>2.559523809523809</v>
+        <v>1.285500747384156</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -991,11 +991,11 @@
         </is>
       </c>
       <c r="C32">
-        <v>4.45</v>
+        <v>2.234977578475336</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1011,11 +1011,11 @@
         </is>
       </c>
       <c r="C33">
-        <v>1.148809523809524</v>
+        <v>0.5769805680119581</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1031,11 +1031,11 @@
         </is>
       </c>
       <c r="C34">
-        <v>4.137755102040816</v>
+        <v>2.078155028827675</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1051,11 +1051,11 @@
         </is>
       </c>
       <c r="C35">
-        <v>1.446428571428571</v>
+        <v>0.726457399103139</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1071,11 +1071,11 @@
         </is>
       </c>
       <c r="C36">
-        <v>4.397959183673469</v>
+        <v>2.208840486867393</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1091,11 +1091,11 @@
         </is>
       </c>
       <c r="C37">
-        <v>1.142857142857143</v>
+        <v>0.5739910313901345</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1111,11 +1111,11 @@
         </is>
       </c>
       <c r="C38">
-        <v>2.806122448979592</v>
+        <v>1.409352978859705</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1131,11 +1131,11 @@
         </is>
       </c>
       <c r="C39">
-        <v>2.377551020408163</v>
+        <v>1.194106342088405</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="C40">
-        <v>5.55</v>
+        <v>2.787443946188341</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1171,11 +1171,11 @@
         </is>
       </c>
       <c r="C41">
-        <v>1.991071428571429</v>
+        <v>1</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1191,11 +1191,11 @@
         </is>
       </c>
       <c r="C42">
-        <v>2.369047619047619</v>
+        <v>1.1898355754858</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="C43">
-        <v>3.602678571428571</v>
+        <v>1.809417040358744</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1231,11 +1231,11 @@
         </is>
       </c>
       <c r="C44">
-        <v>2.899350649350649</v>
+        <v>1.456176110884631</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1251,11 +1251,11 @@
         </is>
       </c>
       <c r="C45">
-        <v>2.128571428571429</v>
+        <v>1.069058295964125</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
         </is>
       </c>
       <c r="C46">
-        <v>0.5285714285714286</v>
+        <v>0.2654708520179372</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1291,11 +1291,11 @@
         </is>
       </c>
       <c r="C47">
-        <v>1.452380952380952</v>
+        <v>0.7294469357249626</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1311,11 +1311,11 @@
         </is>
       </c>
       <c r="C48">
-        <v>2.504464285714286</v>
+        <v>1.257847533632287</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1331,11 +1331,11 @@
         </is>
       </c>
       <c r="C49">
-        <v>1.342857142857143</v>
+        <v>0.6744394618834081</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1351,11 +1351,11 @@
         </is>
       </c>
       <c r="C50">
-        <v>1.816964285714286</v>
+        <v>0.9125560538116592</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
         </is>
       </c>
       <c r="C51">
-        <v>0.5476190476190477</v>
+        <v>0.2750373692077728</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1391,11 +1391,11 @@
         </is>
       </c>
       <c r="C52">
-        <v>1.785714285714286</v>
+        <v>0.8968609865470852</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
         </is>
       </c>
       <c r="C53">
-        <v>5.011904761904762</v>
+        <v>2.517189835575486</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="C54">
-        <v>0.4642857142857143</v>
+        <v>0.2331838565022422</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1451,11 +1451,11 @@
         </is>
       </c>
       <c r="C55">
-        <v>3.030612244897959</v>
+        <v>1.522101217168482</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1471,11 +1471,11 @@
         </is>
       </c>
       <c r="C56">
-        <v>1.821428571428571</v>
+        <v>0.9147982062780269</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1491,11 +1491,11 @@
         </is>
       </c>
       <c r="C57">
-        <v>2.55</v>
+        <v>1.280717488789238</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1511,11 +1511,11 @@
         </is>
       </c>
       <c r="C58">
-        <v>1.135714285714286</v>
+        <v>0.5704035874439461</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="C59">
-        <v>0.5178571428571428</v>
+        <v>0.2600896860986547</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1551,11 +1551,11 @@
         </is>
       </c>
       <c r="C60">
-        <v>1.183673469387755</v>
+        <v>0.5944907110826394</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1571,11 +1571,11 @@
         </is>
       </c>
       <c r="C61">
-        <v>3.901785714285714</v>
+        <v>1.959641255605381</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
         </is>
       </c>
       <c r="C62">
-        <v>5.866071428571429</v>
+        <v>2.946188340807175</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1611,11 +1611,11 @@
         </is>
       </c>
       <c r="C63">
-        <v>1.621428571428571</v>
+        <v>0.8143497757847533</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1631,11 +1631,11 @@
         </is>
       </c>
       <c r="C64">
-        <v>1.485714285714286</v>
+        <v>0.7461883408071749</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1651,11 +1651,11 @@
         </is>
       </c>
       <c r="C65">
-        <v>1.357142857142857</v>
+        <v>0.6816143497757847</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1671,11 +1671,11 @@
         </is>
       </c>
       <c r="C66">
-        <v>2.339285714285714</v>
+        <v>1.174887892376682</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1691,11 +1691,11 @@
         </is>
       </c>
       <c r="C67">
-        <v>3.621428571428571</v>
+        <v>1.818834080717489</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1711,11 +1711,11 @@
         </is>
       </c>
       <c r="C68">
-        <v>1.75</v>
+        <v>0.8789237668161435</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
         </is>
       </c>
       <c r="C69">
-        <v>0.5571428571428572</v>
+        <v>0.2798206278026906</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1751,11 +1751,11 @@
         </is>
       </c>
       <c r="C70">
-        <v>1.535714285714286</v>
+        <v>0.7713004484304933</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1771,11 +1771,11 @@
         </is>
       </c>
       <c r="C71">
-        <v>1.164285714285714</v>
+        <v>0.5847533632286995</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1791,11 +1791,11 @@
         </is>
       </c>
       <c r="C72">
-        <v>2.7</v>
+        <v>1.356053811659193</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1811,11 +1811,11 @@
         </is>
       </c>
       <c r="C73">
-        <v>1.507142857142857</v>
+        <v>0.75695067264574</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1831,11 +1831,11 @@
         </is>
       </c>
       <c r="C74">
-        <v>2.372448979591837</v>
+        <v>1.191543882126842</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
         </is>
       </c>
       <c r="C75">
-        <v>9.107142857142858</v>
+        <v>4.573991031390134</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1871,11 +1871,11 @@
         </is>
       </c>
       <c r="C76">
-        <v>1.779761904761905</v>
+        <v>0.8938714499252616</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1891,11 +1891,11 @@
         </is>
       </c>
       <c r="C77">
-        <v>1.785714285714286</v>
+        <v>0.8968609865470852</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1911,11 +1911,11 @@
         </is>
       </c>
       <c r="C78">
-        <v>3.392857142857143</v>
+        <v>1.704035874439462</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1931,11 +1931,11 @@
         </is>
       </c>
       <c r="C79">
-        <v>1.151785714285714</v>
+        <v>0.57847533632287</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1951,11 +1951,11 @@
         </is>
       </c>
       <c r="C80">
-        <v>2.339285714285714</v>
+        <v>1.174887892376682</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>

</xml_diff>